<commit_message>
added new quadrant data
</commit_message>
<xml_diff>
--- a/data/quadrant/quadrant1_SP_RP_EQUAL.xlsx
+++ b/data/quadrant/quadrant1_SP_RP_EQUAL.xlsx
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.08588330526859</v>
+        <v>0.08588329742263966</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1126138252278397</v>
+        <v>0.1126128921402657</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1416256182909866</v>
+        <v>0.1416248715882232</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -493,13 +493,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08929112920463661</v>
+        <v>0.08929114441299202</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1018532761679925</v>
+        <v>0.1018545815016454</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1354510820214902</v>
+        <v>0.1354520736033861</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -519,13 +519,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.08899395103853536</v>
+        <v>0.08899396700693425</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1016468683144442</v>
+        <v>0.1016481698577618</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1350999968896491</v>
+        <v>0.1351009866694678</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -545,13 +545,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.06073130633801163</v>
+        <v>0.06073125361922211</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1171677704996713</v>
+        <v>0.1171745889883781</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1319718834198597</v>
+        <v>0.1319779128140676</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -571,13 +571,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06083793354910233</v>
+        <v>0.06083788051333652</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1170807597169884</v>
+        <v>0.117087573227652</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1319437700478206</v>
+        <v>0.1319497916242984</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -597,13 +597,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08588135181929531</v>
+        <v>0.08588133505553916</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09940752423234786</v>
+        <v>0.09941624759160034</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1313676614099315</v>
+        <v>0.131374251648168</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08043024139010363</v>
+        <v>0.08043026053774843</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1036777960776089</v>
+        <v>0.1036766823709699</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1312177927324668</v>
+        <v>0.131216924509078</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -649,13 +649,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.08453039774883292</v>
+        <v>0.08453038287866124</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0977569798044399</v>
+        <v>0.09776559275082113</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1292355030324932</v>
+        <v>0.1292420084784064</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.07756245897474132</v>
+        <v>0.07756251986975207</v>
       </c>
       <c r="C10" t="n">
-        <v>0.101704316220831</v>
+        <v>0.1017081010644693</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1279050545528019</v>
+        <v>0.127908101036197</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -701,13 +701,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.07731090618522557</v>
+        <v>0.07731096721671138</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1009860448589967</v>
+        <v>0.1009896864110726</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1271815925023902</v>
+        <v>0.1271845211234064</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -727,13 +727,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.06468472487325112</v>
+        <v>0.0646846850968269</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1023620110495391</v>
+        <v>0.102371931306226</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1210871377894207</v>
+        <v>0.1210955028291402</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.07308701186770478</v>
+        <v>0.07308701050854217</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09592002754302328</v>
+        <v>0.09592728779990474</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1205917202282328</v>
+        <v>0.1205974943758016</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -779,13 +779,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.06382349810933012</v>
+        <v>0.06382346037772409</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1013795954488622</v>
+        <v>0.1013894443213141</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1197967498903315</v>
+        <v>0.1198050646440783</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -805,13 +805,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0727490900875073</v>
+        <v>0.07274908824573457</v>
       </c>
       <c r="C15" t="n">
-        <v>0.09512858737014429</v>
+        <v>0.09513586606067398</v>
       </c>
       <c r="D15" t="n">
-        <v>0.119757581152925</v>
+        <v>0.1197633618921086</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -831,13 +831,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07043222155890612</v>
+        <v>0.07043224705664418</v>
       </c>
       <c r="C16" t="n">
-        <v>0.09475045318166653</v>
+        <v>0.09475366142355186</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1180607733832623</v>
+        <v>0.118063363405492</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -857,13 +857,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07858738034351792</v>
+        <v>0.07858738671328591</v>
       </c>
       <c r="C17" t="n">
-        <v>0.08057022768828144</v>
+        <v>0.08056368564899839</v>
       </c>
       <c r="D17" t="n">
-        <v>0.112550157436577</v>
+        <v>0.1125454787886842</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -883,13 +883,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.03488243112299768</v>
+        <v>0.0348823937511884</v>
       </c>
       <c r="C18" t="n">
-        <v>0.105855459593529</v>
+        <v>0.1058606210548198</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1114547546173241</v>
+        <v>0.1114596450915088</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.03498641313438419</v>
+        <v>0.03498637637921869</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1058008537073576</v>
+        <v>0.1058060921099045</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1114354959122787</v>
+        <v>0.1114404579123666</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -935,13 +935,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.07769766062938577</v>
+        <v>0.07769766861074955</v>
       </c>
       <c r="C20" t="n">
-        <v>0.07982317524529123</v>
+        <v>0.07981670221326713</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1113941909325602</v>
+        <v>0.1113895581270849</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -961,13 +961,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.03071844924805635</v>
+        <v>0.03071842670648588</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08989621502206764</v>
+        <v>0.08990184862159487</v>
       </c>
       <c r="D21" t="n">
-        <v>0.09499975052335261</v>
+        <v>0.09500507420607546</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -987,13 +987,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.07488235793427041</v>
+        <v>0.07488238066439794</v>
       </c>
       <c r="C22" t="n">
-        <v>0.04886246647395333</v>
+        <v>0.04886546455201562</v>
       </c>
       <c r="D22" t="n">
-        <v>0.08941425031679461</v>
+        <v>0.08941590775612633</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1013,13 +1013,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.07369324119440018</v>
+        <v>0.07369326464661191</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04712242120248378</v>
+        <v>0.04712533917234173</v>
       </c>
       <c r="D23" t="n">
-        <v>0.08747123171489203</v>
+        <v>0.0874728234732584</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1039,13 +1039,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.04474304817401594</v>
+        <v>0.04474311680862062</v>
       </c>
       <c r="C24" t="n">
-        <v>0.07248016284177358</v>
+        <v>0.07248326647913302</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0851781331415072</v>
+        <v>0.08518081017010155</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1065,13 +1065,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.04461687795018081</v>
+        <v>0.04461694665067614</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07231593684198329</v>
+        <v>0.07231892755904977</v>
       </c>
       <c r="D25" t="n">
-        <v>0.08497211612849856</v>
+        <v>0.08497469747942836</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1091,13 +1091,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.02758845890528116</v>
+        <v>0.0275884417484716</v>
       </c>
       <c r="C26" t="n">
-        <v>0.07903676620094152</v>
+        <v>0.07904186116584873</v>
       </c>
       <c r="D26" t="n">
-        <v>0.08371340081654</v>
+        <v>0.08371820551510953</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1117,13 +1117,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.01587561814442008</v>
+        <v>0.01587558547882711</v>
       </c>
       <c r="C27" t="n">
-        <v>0.07298678064366931</v>
+        <v>0.07298867616271368</v>
       </c>
       <c r="D27" t="n">
-        <v>0.07469340934911554</v>
+        <v>0.07469525461688335</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1143,13 +1143,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.06903116557960151</v>
+        <v>0.0690311976056254</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02671111699503451</v>
+        <v>0.02670979353463385</v>
       </c>
       <c r="D28" t="n">
-        <v>0.07401881917729289</v>
+        <v>0.0740183714595888</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1169,13 +1169,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.06884281252540893</v>
+        <v>0.06884284427068255</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02628218895269841</v>
+        <v>0.02628086353209221</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07368911922769834</v>
+        <v>0.07368867616716901</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1195,13 +1195,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.03547495533193537</v>
+        <v>0.03547488102947133</v>
       </c>
       <c r="C30" t="n">
-        <v>0.063832908894332</v>
+        <v>0.06384019168546534</v>
       </c>
       <c r="D30" t="n">
-        <v>0.07302816383913058</v>
+        <v>0.073034493621111</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1221,13 +1221,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.03540158384160096</v>
+        <v>0.03540151005697584</v>
       </c>
       <c r="C31" t="n">
-        <v>0.06381648229595677</v>
+        <v>0.06382376447097095</v>
       </c>
       <c r="D31" t="n">
-        <v>0.07297818544691329</v>
+        <v>0.07298451771136215</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1247,13 +1247,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.0390036786492471</v>
+        <v>0.03900362687919676</v>
       </c>
       <c r="C32" t="n">
-        <v>0.05126191069189052</v>
+        <v>0.05126899507545772</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0644132784133605</v>
+        <v>0.06441888516404881</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1273,13 +1273,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.0265756303161902</v>
+        <v>0.02657570539847608</v>
       </c>
       <c r="C33" t="n">
-        <v>0.05540035573097981</v>
+        <v>0.05540025957751547</v>
       </c>
       <c r="D33" t="n">
-        <v>0.06144480077127694</v>
+        <v>0.06144474655072381</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1299,13 +1299,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.02711869822146112</v>
+        <v>0.02711877310160138</v>
       </c>
       <c r="C34" t="n">
-        <v>0.05510193721259903</v>
+        <v>0.0551022343108952</v>
       </c>
       <c r="D34" t="n">
-        <v>0.06141373851027052</v>
+        <v>0.06141403813941023</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1325,13 +1325,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.02432034062440678</v>
+        <v>0.02432035620667341</v>
       </c>
       <c r="C35" t="n">
-        <v>0.05450512607677657</v>
+        <v>0.05450494749310536</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0596849037590954</v>
+        <v>0.05968474702338655</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1351,13 +1351,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.0311995524931039</v>
+        <v>0.03119960131713681</v>
       </c>
       <c r="C36" t="n">
-        <v>0.05021461464400884</v>
+        <v>0.0502128612718016</v>
       </c>
       <c r="D36" t="n">
-        <v>0.05911784501837202</v>
+        <v>0.05911638148135826</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1377,13 +1377,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.03096249396010645</v>
+        <v>0.03096254207812359</v>
       </c>
       <c r="C37" t="n">
-        <v>0.04981512031818995</v>
+        <v>0.04981334873233095</v>
       </c>
       <c r="D37" t="n">
-        <v>0.05865340778288479</v>
+        <v>0.05865192856052042</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1403,13 +1403,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.02737779176604684</v>
+        <v>0.02737781837675919</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0512086115362228</v>
+        <v>0.05120862746746101</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0580677653905572</v>
+        <v>0.05806779198636725</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1429,13 +1429,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.008346969919721508</v>
+        <v>0.008346937460014458</v>
       </c>
       <c r="C39" t="n">
-        <v>0.05524283762719564</v>
+        <v>0.05524393260883437</v>
       </c>
       <c r="D39" t="n">
-        <v>0.05586987574664399</v>
+        <v>0.05587095358995429</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1455,13 +1455,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.02571579373933995</v>
+        <v>0.02571586926743476</v>
       </c>
       <c r="C40" t="n">
-        <v>0.04403633726031895</v>
+        <v>0.04403525450269997</v>
       </c>
       <c r="D40" t="n">
-        <v>0.05099510806880236</v>
+        <v>0.05099421115477083</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1481,13 +1481,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.03885349241380226</v>
+        <v>0.03885348872598964</v>
       </c>
       <c r="C41" t="n">
-        <v>0.003933007477605287</v>
+        <v>0.003929828402121042</v>
       </c>
       <c r="D41" t="n">
-        <v>0.03905204758483592</v>
+        <v>0.03905172387297034</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1503,13 +1503,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.01081036743550564</v>
+        <v>0.01081030821760454</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0337698776422458</v>
+        <v>0.03377184431399964</v>
       </c>
       <c r="D42" t="n">
-        <v>0.03545798471519347</v>
+        <v>0.03545983970816335</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1529,13 +1529,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.02041753048945074</v>
+        <v>0.02041753177960865</v>
       </c>
       <c r="C43" t="n">
-        <v>0.02890365292605957</v>
+        <v>0.0289095951681515</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03538780444952417</v>
+        <v>0.03539265879752097</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1555,13 +1555,13 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.0104459035321001</v>
+        <v>0.01044584510556036</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03297389086570605</v>
+        <v>0.03297581119725537</v>
       </c>
       <c r="D44" t="n">
-        <v>0.03458893434937587</v>
+        <v>0.0345907473768115</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1581,13 +1581,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.02576076756921553</v>
+        <v>0.02576079430406898</v>
       </c>
       <c r="C45" t="n">
-        <v>0.0007885895862724308</v>
+        <v>0.0007862710885109629</v>
       </c>
       <c r="D45" t="n">
-        <v>0.02577283490985661</v>
+        <v>0.02577279079574389</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1607,13 +1607,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.002112302171463022</v>
+        <v>0.002112272327707286</v>
       </c>
       <c r="C46" t="n">
-        <v>0.02243134669294164</v>
+        <v>0.02243195691745916</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02253058221445933</v>
+        <v>0.02253118695349053</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1633,13 +1633,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.005531458351967645</v>
+        <v>0.005531493246869912</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01899485604944792</v>
+        <v>0.01899228961995462</v>
       </c>
       <c r="D47" t="n">
-        <v>0.01978387191221174</v>
+        <v>0.01978141760714847</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1659,13 +1659,13 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.008796223132089366</v>
+        <v>0.008796236113647393</v>
       </c>
       <c r="C48" t="n">
-        <v>0.01769201177816282</v>
+        <v>0.01769375958209627</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0197580571450777</v>
+        <v>0.01975962798020393</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1685,13 +1685,13 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.005288689236892901</v>
+        <v>0.005288724862033058</v>
       </c>
       <c r="C49" t="n">
-        <v>0.01871280694371555</v>
+        <v>0.01871023528792063</v>
       </c>
       <c r="D49" t="n">
-        <v>0.01944580616886828</v>
+        <v>0.01944334115309498</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1711,13 +1711,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.007612416751933826</v>
+        <v>0.007612367974104162</v>
       </c>
       <c r="C50" t="n">
-        <v>0.009123839400591397</v>
+        <v>0.009152647705836511</v>
       </c>
       <c r="D50" t="n">
-        <v>0.01188248013728223</v>
+        <v>0.01190458341145632</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1737,13 +1737,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.007541840881792798</v>
+        <v>0.007541792680853372</v>
       </c>
       <c r="C51" t="n">
-        <v>0.008987612629173991</v>
+        <v>0.00901630066851017</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01173271258739295</v>
+        <v>0.01175467203225809</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1763,13 +1763,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.00499713207953843</v>
+        <v>0.004997105875763457</v>
       </c>
       <c r="C52" t="n">
-        <v>0.006880677151286842</v>
+        <v>0.006880583214465535</v>
       </c>
       <c r="D52" t="n">
-        <v>0.008503825438036277</v>
+        <v>0.008503734033045399</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1789,13 +1789,13 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.00139026699353601</v>
+        <v>0.00139024605353247</v>
       </c>
       <c r="C53" t="n">
-        <v>0.005944299000113893</v>
+        <v>0.005950188323006304</v>
       </c>
       <c r="D53" t="n">
-        <v>0.006104713991340682</v>
+        <v>0.006110443942022804</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1815,13 +1815,13 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.004323232217261869</v>
+        <v>0.00432325294348684</v>
       </c>
       <c r="C54" t="n">
-        <v>0.003286896088223008</v>
+        <v>0.003279641527890246</v>
       </c>
       <c r="D54" t="n">
-        <v>0.005430839962579148</v>
+        <v>0.005426468885456719</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1841,13 +1841,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.004427899093397457</v>
+        <v>0.004427852045893376</v>
       </c>
       <c r="C55" t="n">
-        <v>0.001070414639620285</v>
+        <v>0.001070715693449697</v>
       </c>
       <c r="D55" t="n">
-        <v>0.004555444861045236</v>
+        <v>0.004555469880980624</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1867,13 +1867,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.001298056288289769</v>
+        <v>0.001298069416368812</v>
       </c>
       <c r="C56" t="n">
-        <v>0.001772373168314923</v>
+        <v>0.001766043160256153</v>
       </c>
       <c r="D56" t="n">
-        <v>0.002196874319420956</v>
+        <v>0.002191778422560001</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1893,13 +1893,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.00201750367724995</v>
+        <v>0.002017507081386075</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0005686840953467191</v>
+        <v>0.0005667778846154517</v>
       </c>
       <c r="D57" t="n">
-        <v>0.002096120866748238</v>
+        <v>0.002095607786283523</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1919,13 +1919,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.000275268433404305</v>
+        <v>0.0002752815688581456</v>
       </c>
       <c r="C58" t="n">
-        <v>0.001706934682254155</v>
+        <v>0.001700762372943131</v>
       </c>
       <c r="D58" t="n">
-        <v>0.00172898777321037</v>
+        <v>0.001722896570131868</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
updated analysis w streamlit
</commit_message>
<xml_diff>
--- a/data/quadrant/quadrant1_SP_RP_EQUAL.xlsx
+++ b/data/quadrant/quadrant1_SP_RP_EQUAL.xlsx
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.08588329742263966</v>
+        <v>0.08588332064103023</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1126128921402657</v>
+        <v>0.1126149353329733</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1416248715882232</v>
+        <v>0.1416265103163238</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -493,13 +493,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08929114441299202</v>
+        <v>0.08929118420888102</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1018545815016454</v>
+        <v>0.101857234125417</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1354520736033861</v>
+        <v>0.1354540945158335</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -519,13 +519,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.08899396700693425</v>
+        <v>0.08899401048283469</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1016481698577618</v>
+        <v>0.1016509492814966</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1351009866694678</v>
+        <v>0.1351031065210874</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -545,13 +545,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.06073125361922211</v>
+        <v>0.06073129316736296</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1171745889883781</v>
+        <v>0.1171663963776744</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1319779128140676</v>
+        <v>0.1319706573822776</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -571,13 +571,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06083788051333652</v>
+        <v>0.0608379168399362</v>
       </c>
       <c r="C6" t="n">
-        <v>0.117087573227652</v>
+        <v>0.1170793116193844</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1319497916242984</v>
+        <v>0.1319424773706023</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -597,13 +597,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08588133505553916</v>
+        <v>0.08588138363330745</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09941624759160034</v>
+        <v>0.09940781665928777</v>
       </c>
       <c r="D7" t="n">
-        <v>0.131374251648168</v>
+        <v>0.1313679034914461</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08043026053774843</v>
+        <v>0.08043029690219729</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1036766823709699</v>
+        <v>0.1036811754135831</v>
       </c>
       <c r="D8" t="n">
-        <v>0.131216924509078</v>
+        <v>0.1312204968551704</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -649,13 +649,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.08453038287866124</v>
+        <v>0.08453042923926318</v>
       </c>
       <c r="C9" t="n">
-        <v>0.09776559275082113</v>
+        <v>0.09775728516034188</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1292420084784064</v>
+        <v>0.1292357546087555</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.07756251986975207</v>
+        <v>0.07756254439034889</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1017081010644693</v>
+        <v>0.1017096795003943</v>
       </c>
       <c r="D10" t="n">
-        <v>0.127908101036197</v>
+        <v>0.1279093710264333</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -701,13 +701,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.07731096721671138</v>
+        <v>0.07731098865864601</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1009896864110726</v>
+        <v>0.1009912011297902</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1271845211234064</v>
+        <v>0.1271857369087235</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -727,13 +727,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0646846850968269</v>
+        <v>0.06468475557242054</v>
       </c>
       <c r="C12" t="n">
-        <v>0.102371931306226</v>
+        <v>0.1023620916296421</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1210955028291402</v>
+        <v>0.1210872223079671</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.07308701050854217</v>
+        <v>0.07308705776607458</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09592728779990474</v>
+        <v>0.09592130013042781</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1205974943758016</v>
+        <v>0.1205927602786052</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -779,13 +779,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.06382346037772409</v>
+        <v>0.06382352732180137</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1013894443213141</v>
+        <v>0.1013797013576453</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1198050646440783</v>
+        <v>0.1197968550804322</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -805,13 +805,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.07274908824573457</v>
+        <v>0.07274913395406939</v>
       </c>
       <c r="C15" t="n">
-        <v>0.09513586606067398</v>
+        <v>0.09512976447202832</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1197633618921086</v>
+        <v>0.119758542825014</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -831,13 +831,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07043224705664418</v>
+        <v>0.07043226192560946</v>
       </c>
       <c r="C16" t="n">
-        <v>0.09475366142355186</v>
+        <v>0.09475371213092773</v>
       </c>
       <c r="D16" t="n">
-        <v>0.118063363405492</v>
+        <v>0.118063412971794</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -857,13 +857,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07858738671328591</v>
+        <v>0.07858733415069197</v>
       </c>
       <c r="C17" t="n">
-        <v>0.08056368564899839</v>
+        <v>0.08056650515104753</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1125454787886842</v>
+        <v>0.1125474603941212</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -883,13 +883,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0348823937511884</v>
+        <v>0.03488245248694007</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1058606210548198</v>
+        <v>0.1058611459854738</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1114596450915088</v>
+        <v>0.1114601620349685</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.03498637637921869</v>
+        <v>0.03498643538402768</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1058060921099045</v>
+        <v>0.1058065626826635</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1114404579123666</v>
+        <v>0.1114409232176455</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -935,13 +935,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.07769766861074955</v>
+        <v>0.07769762097629454</v>
       </c>
       <c r="C20" t="n">
-        <v>0.07981670221326713</v>
+        <v>0.079819671430856</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1113895581270849</v>
+        <v>0.1113916525270441</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -961,13 +961,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.03071842670648588</v>
+        <v>0.03071845680106956</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08990184862159487</v>
+        <v>0.08989986858235997</v>
       </c>
       <c r="D21" t="n">
-        <v>0.09500507420607546</v>
+        <v>0.09500321025820532</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -987,13 +987,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.07488238066439794</v>
+        <v>0.07488237640623181</v>
       </c>
       <c r="C22" t="n">
-        <v>0.04886546455201562</v>
+        <v>0.04886291357764667</v>
       </c>
       <c r="D22" t="n">
-        <v>0.08941590775612633</v>
+        <v>0.08941451011743648</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1013,13 +1013,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.07369326464661191</v>
+        <v>0.07369326094406196</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04712533917234173</v>
+        <v>0.04712286256433682</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0874728234732584</v>
+        <v>0.08747148612449079</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1039,13 +1039,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.04474311680862062</v>
+        <v>0.04474313230199212</v>
       </c>
       <c r="C24" t="n">
-        <v>0.07248326647913302</v>
+        <v>0.07248571670905528</v>
       </c>
       <c r="D24" t="n">
-        <v>0.08518081017010155</v>
+        <v>0.08518290330235866</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1065,13 +1065,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.04461694665067614</v>
+        <v>0.04461696058254975</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07231892755904977</v>
+        <v>0.07232133092463733</v>
       </c>
       <c r="D25" t="n">
-        <v>0.08497469747942836</v>
+        <v>0.08497675022225609</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1091,13 +1091,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.0275884417484716</v>
+        <v>0.02758846592293456</v>
       </c>
       <c r="C26" t="n">
-        <v>0.07904186116584873</v>
+        <v>0.07904062167515934</v>
       </c>
       <c r="D26" t="n">
-        <v>0.08371820551510953</v>
+        <v>0.08371704322762832</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1117,13 +1117,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.01587558547882711</v>
+        <v>0.01587562420176378</v>
       </c>
       <c r="C27" t="n">
-        <v>0.07298867616271368</v>
+        <v>0.07299009080835227</v>
       </c>
       <c r="D27" t="n">
-        <v>0.07469525461688335</v>
+        <v>0.07469664517237129</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1143,13 +1143,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.0690311976056254</v>
+        <v>0.06903115274358496</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02670979353463385</v>
+        <v>0.02671064665878612</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0740183714595888</v>
+        <v>0.07401863747758856</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1169,13 +1169,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.06884284427068255</v>
+        <v>0.06884279897239383</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02628086353209221</v>
+        <v>0.02628168407793422</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07368867616716901</v>
+        <v>0.07368892649730874</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1195,13 +1195,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.03547488102947133</v>
+        <v>0.03547490017167763</v>
       </c>
       <c r="C30" t="n">
-        <v>0.06384019168546534</v>
+        <v>0.06382849840505711</v>
       </c>
       <c r="D30" t="n">
-        <v>0.073034493621111</v>
+        <v>0.07302428192618447</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1221,13 +1221,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.03540151005697584</v>
+        <v>0.03540153181287879</v>
       </c>
       <c r="C31" t="n">
-        <v>0.06382376447097095</v>
+        <v>0.0638121367742561</v>
       </c>
       <c r="D31" t="n">
-        <v>0.07298451771136215</v>
+        <v>0.07297436025341117</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1247,13 +1247,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.03900362687919676</v>
+        <v>0.03900367308630602</v>
       </c>
       <c r="C32" t="n">
-        <v>0.05126899507545772</v>
+        <v>0.05125930398553191</v>
       </c>
       <c r="D32" t="n">
-        <v>0.06441888516404881</v>
+        <v>0.0644112005733832</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1273,13 +1273,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.02657570539847608</v>
+        <v>0.02657566832637107</v>
       </c>
       <c r="C33" t="n">
-        <v>0.05540025957751547</v>
+        <v>0.05540307554476235</v>
       </c>
       <c r="D33" t="n">
-        <v>0.06144474655072381</v>
+        <v>0.0614472694821497</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1299,13 +1299,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.02711877310160138</v>
+        <v>0.02711873523525138</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0551022343108952</v>
+        <v>0.05510478699972096</v>
       </c>
       <c r="D34" t="n">
-        <v>0.06141403813941023</v>
+        <v>0.0614163117668611</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1325,13 +1325,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.02432035620667341</v>
+        <v>0.02432036016320607</v>
       </c>
       <c r="C35" t="n">
-        <v>0.05450494749310536</v>
+        <v>0.05450754626598295</v>
       </c>
       <c r="D35" t="n">
-        <v>0.05968474702338655</v>
+        <v>0.05968712188074018</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1351,13 +1351,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.03119960131713681</v>
+        <v>0.03119958627222988</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0502128612718016</v>
+        <v>0.05021704664887276</v>
       </c>
       <c r="D36" t="n">
-        <v>0.05911638148135826</v>
+        <v>0.05911992860020535</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1377,13 +1377,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.03096254207812359</v>
+        <v>0.03096252320744195</v>
       </c>
       <c r="C37" t="n">
-        <v>0.04981334873233095</v>
+        <v>0.04981743222110632</v>
       </c>
       <c r="D37" t="n">
-        <v>0.05865192856052042</v>
+        <v>0.05865538676435357</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1403,13 +1403,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.02737781837675919</v>
+        <v>0.02737779775200264</v>
       </c>
       <c r="C38" t="n">
-        <v>0.05120862746746101</v>
+        <v>0.05121036617202294</v>
       </c>
       <c r="D38" t="n">
-        <v>0.05806779198636725</v>
+        <v>0.05806931559112982</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1429,13 +1429,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.008346937460014458</v>
+        <v>0.008346966531183121</v>
       </c>
       <c r="C39" t="n">
-        <v>0.05524393260883437</v>
+        <v>0.05524551099066516</v>
       </c>
       <c r="D39" t="n">
-        <v>0.05587095358995429</v>
+        <v>0.05587251860165601</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1455,13 +1455,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.02571586926743476</v>
+        <v>0.02571585119736951</v>
       </c>
       <c r="C40" t="n">
-        <v>0.04403525450269997</v>
+        <v>0.04404174538154301</v>
       </c>
       <c r="D40" t="n">
-        <v>0.05099421115477083</v>
+        <v>0.05099980724530158</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1481,13 +1481,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.03885348872598964</v>
+        <v>0.03885345098247834</v>
       </c>
       <c r="C41" t="n">
-        <v>0.003929828402121042</v>
+        <v>0.00393351929377147</v>
       </c>
       <c r="D41" t="n">
-        <v>0.03905172387297034</v>
+        <v>0.03905205791353791</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1503,13 +1503,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.01081030821760454</v>
+        <v>0.01081033177561329</v>
       </c>
       <c r="C42" t="n">
-        <v>0.03377184431399964</v>
+        <v>0.03376725432254058</v>
       </c>
       <c r="D42" t="n">
-        <v>0.03545983970816335</v>
+        <v>0.03545547542456552</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1529,13 +1529,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.02041753177960865</v>
+        <v>0.02041759736177141</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0289095951681515</v>
+        <v>0.02890840381462799</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03539265879752097</v>
+        <v>0.03539172351181859</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1555,13 +1555,13 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.01044584510556036</v>
+        <v>0.01044587000876794</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03297581119725537</v>
+        <v>0.03297126211336516</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0345907473768115</v>
+        <v>0.03458641822433058</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1581,13 +1581,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.02576079430406898</v>
+        <v>0.02576082034745903</v>
       </c>
       <c r="C45" t="n">
-        <v>0.0007862710885109629</v>
+        <v>0.0007874562591249093</v>
       </c>
       <c r="D45" t="n">
-        <v>0.02577279079574389</v>
+        <v>0.02577285301114516</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1607,13 +1607,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.002112272327707286</v>
+        <v>0.002112293504052024</v>
       </c>
       <c r="C46" t="n">
-        <v>0.02243195691745916</v>
+        <v>0.02242766117759908</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02253118695349053</v>
+        <v>0.02252691212182543</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1633,13 +1633,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.005531493246869912</v>
+        <v>0.005531485563922686</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01899228961995462</v>
+        <v>0.01899047726851169</v>
       </c>
       <c r="D47" t="n">
-        <v>0.01978141760714847</v>
+        <v>0.01977967541264882</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1659,13 +1659,13 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.008796236113647393</v>
+        <v>0.008796166297941745</v>
       </c>
       <c r="C48" t="n">
-        <v>0.01769375958209627</v>
+        <v>0.0176920949741046</v>
       </c>
       <c r="D48" t="n">
-        <v>0.01975962798020393</v>
+        <v>0.01975810633926702</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1685,13 +1685,13 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.005288724862033058</v>
+        <v>0.005288720583241264</v>
       </c>
       <c r="C49" t="n">
-        <v>0.01871023528792063</v>
+        <v>0.01870849008552329</v>
       </c>
       <c r="D49" t="n">
-        <v>0.01944334115309498</v>
+        <v>0.0194416605949112</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1711,13 +1711,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.007612367974104162</v>
+        <v>0.007612535682187564</v>
       </c>
       <c r="C50" t="n">
-        <v>0.009152647705836511</v>
+        <v>0.009151425068063254</v>
       </c>
       <c r="D50" t="n">
-        <v>0.01190458341145632</v>
+        <v>0.01190375068156904</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1737,13 +1737,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.007541792680853372</v>
+        <v>0.007541960567385532</v>
       </c>
       <c r="C51" t="n">
-        <v>0.00901630066851017</v>
+        <v>0.009015128652301573</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01175467203225809</v>
+        <v>0.0117538807981682</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1763,13 +1763,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.004997105875763457</v>
+        <v>0.004997101473531156</v>
       </c>
       <c r="C52" t="n">
-        <v>0.006880583214465535</v>
+        <v>0.006877888236938441</v>
       </c>
       <c r="D52" t="n">
-        <v>0.008503734033045399</v>
+        <v>0.008501551019466003</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1789,13 +1789,13 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.00139024605353247</v>
+        <v>0.001390263691353682</v>
       </c>
       <c r="C53" t="n">
-        <v>0.005950188323006304</v>
+        <v>0.005949458780568908</v>
       </c>
       <c r="D53" t="n">
-        <v>0.006110443942022804</v>
+        <v>0.006109737548633725</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1815,13 +1815,13 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.00432325294348684</v>
+        <v>0.00432328809162941</v>
       </c>
       <c r="C54" t="n">
-        <v>0.003279641527890246</v>
+        <v>0.003293067748256011</v>
       </c>
       <c r="D54" t="n">
-        <v>0.005426468885456719</v>
+        <v>0.005434621892811732</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1841,13 +1841,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.004427852045893376</v>
+        <v>0.004427918706507529</v>
       </c>
       <c r="C55" t="n">
-        <v>0.001070715693449697</v>
+        <v>0.001065788224361497</v>
       </c>
       <c r="D55" t="n">
-        <v>0.004555469880980624</v>
+        <v>0.004554379058733138</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1867,13 +1867,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.001298069416368812</v>
+        <v>0.001298149756997882</v>
       </c>
       <c r="C56" t="n">
-        <v>0.001766043160256153</v>
+        <v>0.001771772453070957</v>
       </c>
       <c r="D56" t="n">
-        <v>0.002191778422560001</v>
+        <v>0.002196444949698202</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1893,13 +1893,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.002017507081386075</v>
+        <v>0.002017540445536828</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0005667778846154517</v>
+        <v>0.0005682484791271444</v>
       </c>
       <c r="D57" t="n">
-        <v>0.002095607786283523</v>
+        <v>0.002096038115924244</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1919,13 +1919,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0002752815688581456</v>
+        <v>0.0002753543240264799</v>
       </c>
       <c r="C58" t="n">
-        <v>0.001700762372943131</v>
+        <v>0.001706504031273712</v>
       </c>
       <c r="D58" t="n">
-        <v>0.001722896570131868</v>
+        <v>0.001728576296410867</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>

</xml_diff>